<commit_message>
fix: fixed missing options in ocg course data
</commit_message>
<xml_diff>
--- a/cs-faker-data-provider/data/foggia-exercise-80ab809d-0539-4980-9f9c-0d46252761b1.xlsx
+++ b/cs-faker-data-provider/data/foggia-exercise-80ab809d-0539-4980-9f9c-0d46252761b1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Case</t>
   </si>
@@ -158,15 +158,30 @@
 aggiungere o reagire ai messaggi degli altri!</t>
   </si>
   <si>
-    <t>Processo di registrazione/accesso</t>
-  </si>
-  <si>
-    <t>1) Crea un nuovo account sulla piattaforma di apprendimento:
-https://learn.icdl.at/login/signup.php (o accedi se hai già un account: https://learn.icdl.at/login/index.php )</t>
-  </si>
-  <si>
-    <t>2) Accedi al corso: dopo l&amp;#39;iscrizione, il corso apparirà sulla tua dashboard nella piattaforma di
-apprendimento (https://learn.icdl.at/) e sarà possibile accedervi da lì.</t>
+    <t>Procedura di registrazione (solo per la prima volta)</t>
+  </si>
+  <si>
+    <t>1) Crea un nuovo account sulla piattaforma di apprendimento: https://learn.ocg.at/login/signup.php</t>
+  </si>
+  <si>
+    <t>2) Una volta creato l&amp;#39;account, riceverai un&amp;#39;email con un link per confermare l&amp;#39;account
+(controlla la cartella spam)</t>
+  </si>
+  <si>
+    <t>3) Dopo aver creato un account per la piattaforma di apprendimento, devi iscriverti al corso.
+Puoi farlo utilizzando questo collegamento: https://learn.ocg.at/user/index.php?id=23. La
+password per questa autoiscrizione è: mj3poqx7nvKY</t>
+  </si>
+  <si>
+    <t>4) Dopo l&amp;#39;iscrizione, il corso apparirà sulla tua dashboard nella piattaforma di
+apprendimento e sarà possibile accedervi da lì.</t>
+  </si>
+  <si>
+    <t>Registrazione</t>
+  </si>
+  <si>
+    <t>Dopo aver completato questi passaggi la prima volta, puoi effettuare il login e accedere al
+materiale tramite questo collegamento: https://learn.ocg.at/login/index.php</t>
   </si>
   <si>
     <t>Link ai materiali didattici</t>
@@ -178,7 +193,8 @@
     <t>Domande riflessive</t>
   </si>
   <si>
-    <t>Dopo aver terminato il capitolo, rispondi a queste domande in uno o più post in questo canale</t>
+    <t>Dopo aver terminato il capitolo, rispondi a queste domande in uno o più post in questo
+canale.</t>
   </si>
   <si>
     <t>1. Quanto è stato rilevante questo modulo per la tua pratica lavorativa?
@@ -206,7 +222,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,12 +246,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -310,7 +320,7 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -319,10 +329,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -737,10 +747,18 @@
       <c r="Q1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
+      <c r="R1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="V1" s="7"/>
       <c r="W1" s="7"/>
       <c r="X1" s="13"/>

</xml_diff>